<commit_message>
Added setters and calc class
</commit_message>
<xml_diff>
--- a/Data/Skyhawk_Attributes.xlsx
+++ b/Data/Skyhawk_Attributes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fernando\Documents\Python_Practice\Skyhawk Modeling\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fernando\Documents\Python_Practice\Skyhawk_Modeling\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89FDDF77-4BED-40F6-8938-2A921842594F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A64CA0B-6808-4EBB-9648-25BE85E8F706}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4404" yWindow="1764" windowWidth="17280" windowHeight="9072" xr2:uid="{F4B4ECF7-3D9A-4A2A-93FB-7EEC8523274B}"/>
+    <workbookView xWindow="1104" yWindow="2484" windowWidth="6972" windowHeight="9072" xr2:uid="{F4B4ECF7-3D9A-4A2A-93FB-7EEC8523274B}"/>
   </bookViews>
   <sheets>
     <sheet name="Attributes" sheetId="1" r:id="rId1"/>
@@ -33,15 +33,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
-    <t>Wing Area m^2</t>
-  </si>
-  <si>
-    <t>Wing Span m</t>
-  </si>
-  <si>
-    <t>mass kg</t>
-  </si>
-  <si>
     <t>Ixx</t>
   </si>
   <si>
@@ -79,6 +70,15 @@
   </si>
   <si>
     <t>cnr</t>
+  </si>
+  <si>
+    <t>mass</t>
+  </si>
+  <si>
+    <t>wingarea</t>
+  </si>
+  <si>
+    <t>span</t>
   </si>
 </sst>
 </file>
@@ -433,7 +433,7 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -444,55 +444,55 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
       <c r="Q1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Simulation is more accurate now,but still off
</commit_message>
<xml_diff>
--- a/Data/Skyhawk_Attributes.xlsx
+++ b/Data/Skyhawk_Attributes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fernando\Documents\Python_Practice\Skyhawk_Modeling\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A64CA0B-6808-4EBB-9648-25BE85E8F706}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC614F41-7A52-4819-B5E6-572564C33624}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1104" yWindow="2484" windowWidth="6972" windowHeight="9072" xr2:uid="{F4B4ECF7-3D9A-4A2A-93FB-7EEC8523274B}"/>
+    <workbookView xWindow="7128" yWindow="3252" windowWidth="12636" windowHeight="9072" xr2:uid="{F4B4ECF7-3D9A-4A2A-93FB-7EEC8523274B}"/>
   </bookViews>
   <sheets>
     <sheet name="Attributes" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Ixx</t>
   </si>
@@ -60,9 +60,6 @@
     <t>clr</t>
   </si>
   <si>
-    <t>cdr</t>
-  </si>
-  <si>
     <t>cnb</t>
   </si>
   <si>
@@ -79,6 +76,12 @@
   </si>
   <si>
     <t>span</t>
+  </si>
+  <si>
+    <t>cldr</t>
+  </si>
+  <si>
+    <t>cndr</t>
   </si>
 </sst>
 </file>
@@ -432,8 +435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54934CBA-3354-47A3-B18B-731A01AE50C0}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -444,13 +447,13 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
-        <v>15</v>
-      </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -480,19 +483,19 @@
         <v>8</v>
       </c>
       <c r="M1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>11</v>
       </c>
-      <c r="P1" t="s">
-        <v>12</v>
-      </c>
       <c r="Q1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
@@ -530,13 +533,13 @@
         <v>-0.25</v>
       </c>
       <c r="L2">
-        <v>0.16</v>
+        <v>0.03</v>
       </c>
       <c r="M2">
         <v>0.04</v>
       </c>
       <c r="N2">
-        <v>0.26</v>
+        <v>0.1</v>
       </c>
       <c r="O2">
         <v>2.5000000000000001E-2</v>

</xml_diff>

<commit_message>
Organized Classes and created dedicated main
</commit_message>
<xml_diff>
--- a/Data/Skyhawk_Attributes.xlsx
+++ b/Data/Skyhawk_Attributes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fernando\Documents\Python_Practice\Skyhawk_Modeling\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC614F41-7A52-4819-B5E6-572564C33624}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427E1A78-67CB-4312-9582-17C32B38F5AD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7128" yWindow="3252" windowWidth="12636" windowHeight="9072" xr2:uid="{F4B4ECF7-3D9A-4A2A-93FB-7EEC8523274B}"/>
+    <workbookView xWindow="10080" yWindow="2856" windowWidth="12636" windowHeight="9072" xr2:uid="{F4B4ECF7-3D9A-4A2A-93FB-7EEC8523274B}"/>
   </bookViews>
   <sheets>
     <sheet name="Attributes" sheetId="1" r:id="rId1"/>
@@ -436,7 +436,7 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added Control System Plot
</commit_message>
<xml_diff>
--- a/Data/Skyhawk_Attributes.xlsx
+++ b/Data/Skyhawk_Attributes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fernando\Documents\Python_Practice\Skyhawk_Modeling\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{427E1A78-67CB-4312-9582-17C32B38F5AD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68B229A-35F9-45F2-94C1-8DF4CB60CC2D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10080" yWindow="2856" windowWidth="12636" windowHeight="9072" xr2:uid="{F4B4ECF7-3D9A-4A2A-93FB-7EEC8523274B}"/>
+    <workbookView xWindow="8808" yWindow="2052" windowWidth="12096" windowHeight="9072" xr2:uid="{F4B4ECF7-3D9A-4A2A-93FB-7EEC8523274B}"/>
   </bookViews>
   <sheets>
     <sheet name="Attributes" sheetId="1" r:id="rId1"/>
@@ -436,7 +436,7 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -533,13 +533,13 @@
         <v>-0.25</v>
       </c>
       <c r="L2">
-        <v>0.03</v>
+        <v>0.16</v>
       </c>
       <c r="M2">
         <v>0.04</v>
       </c>
       <c r="N2">
-        <v>0.1</v>
+        <v>0.26</v>
       </c>
       <c r="O2">
         <v>2.5000000000000001E-2</v>

</xml_diff>